<commit_message>
Fix \n into doc_id. run again validation notebooks
</commit_message>
<xml_diff>
--- a/code/outputs/misaligned_similarity.xlsx
+++ b/code/outputs/misaligned_similarity.xlsx
@@ -136,22 +136,22 @@
     <t>documents-2024-12-02-5.json</t>
   </si>
   <si>
+    <t>documents-2024-11-30-1.json</t>
+  </si>
+  <si>
+    <t>documents-2024-11-30-2.json</t>
+  </si>
+  <si>
+    <t>documents-2024-12-01-1.json</t>
+  </si>
+  <si>
+    <t>documents-2024-12-02-1.json</t>
+  </si>
+  <si>
+    <t>documents-2024-12-02-9.json</t>
+  </si>
+  <si>
     <t>documents-2024-12-02-8.json</t>
-  </si>
-  <si>
-    <t>documents-2024-12-02-9.json</t>
-  </si>
-  <si>
-    <t>documents-2024-11-30-1.json</t>
-  </si>
-  <si>
-    <t>documents-2024-11-30-2.json</t>
-  </si>
-  <si>
-    <t>documents-2024-12-01-1.json</t>
-  </si>
-  <si>
-    <t>documents-2024-12-02-1.json</t>
   </si>
   <si>
     <t>documents-2024-12-02-6.json</t>
@@ -1061,7 +1061,7 @@
         <v>27</v>
       </c>
       <c r="H9" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="I9" t="s">
         <v>52</v>
@@ -1117,7 +1117,7 @@
         <v>27</v>
       </c>
       <c r="H10" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="I10" t="s">
         <v>52</v>
@@ -1397,7 +1397,7 @@
         <v>30</v>
       </c>
       <c r="H15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I15" t="s">
         <v>55</v>
@@ -1453,7 +1453,7 @@
         <v>30</v>
       </c>
       <c r="H16" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="I16" t="s">
         <v>55</v>
@@ -1491,7 +1491,7 @@
         <v>20</v>
       </c>
       <c r="B17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C17">
         <v>4</v>
@@ -1509,7 +1509,7 @@
         <v>30</v>
       </c>
       <c r="H17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I17" t="s">
         <v>55</v>
@@ -1536,10 +1536,10 @@
         <v>69</v>
       </c>
       <c r="Q17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:18">
@@ -1547,7 +1547,7 @@
         <v>20</v>
       </c>
       <c r="B18">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C18">
         <v>4</v>
@@ -1565,7 +1565,7 @@
         <v>30</v>
       </c>
       <c r="H18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I18" t="s">
         <v>55</v>
@@ -1592,10 +1592,10 @@
         <v>69</v>
       </c>
       <c r="Q18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R18" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:18">
@@ -1621,7 +1621,7 @@
         <v>30</v>
       </c>
       <c r="H19" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I19" t="s">
         <v>55</v>
@@ -1677,7 +1677,7 @@
         <v>30</v>
       </c>
       <c r="H20" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I20" t="s">
         <v>55</v>
@@ -1733,7 +1733,7 @@
         <v>30</v>
       </c>
       <c r="H21" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I21" t="s">
         <v>55</v>
@@ -1845,7 +1845,7 @@
         <v>32</v>
       </c>
       <c r="H23" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="I23" t="s">
         <v>57</v>
@@ -1901,7 +1901,7 @@
         <v>32</v>
       </c>
       <c r="H24" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="I24" t="s">
         <v>58</v>
@@ -1957,7 +1957,7 @@
         <v>32</v>
       </c>
       <c r="H25" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="I25" t="s">
         <v>58</v>
@@ -2013,7 +2013,7 @@
         <v>32</v>
       </c>
       <c r="H26" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="I26" t="s">
         <v>58</v>
@@ -2069,7 +2069,7 @@
         <v>32</v>
       </c>
       <c r="H27" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="I27" t="s">
         <v>58</v>
@@ -2125,7 +2125,7 @@
         <v>37</v>
       </c>
       <c r="H28" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I28" t="s">
         <v>59</v>
@@ -2237,7 +2237,7 @@
         <v>34</v>
       </c>
       <c r="H30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I30" t="s">
         <v>60</v>
@@ -2293,7 +2293,7 @@
         <v>34</v>
       </c>
       <c r="H31" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="I31" t="s">
         <v>60</v>

</xml_diff>

<commit_message>
run_v5 and GUI improvements
</commit_message>
<xml_diff>
--- a/code/outputs/misaligned_similarity.xlsx
+++ b/code/outputs/misaligned_similarity.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="63">
   <si>
     <t>doc_id</t>
   </si>
@@ -73,12 +73,12 @@
     <t>§ 275.0-5</t>
   </si>
   <si>
+    <t>§ 275.0-7</t>
+  </si>
+  <si>
     <t>§ 275.0-2</t>
   </si>
   <si>
-    <t>§ 275.0-7</t>
-  </si>
-  <si>
     <t>Operative Rule</t>
   </si>
   <si>
@@ -88,21 +88,12 @@
     <t>§ 275.0-5['(c)(2)']</t>
   </si>
   <si>
-    <t>§ 275.0-2['(b)(2)(i)']</t>
-  </si>
-  <si>
-    <t>§ 275.0-2['(b)(2)(ii)']</t>
-  </si>
-  <si>
     <t>§ 275.0-5['(c)(1)']</t>
   </si>
   <si>
     <t>§ 275.0-7['(a)(1)']</t>
   </si>
   <si>
-    <t>§ 275.0-2['(b)(2)(iii)']</t>
-  </si>
-  <si>
     <t>§ 275.0-7['(a)']</t>
   </si>
   <si>
@@ -121,75 +112,66 @@
     <t>§ 275.0-5['(c)']</t>
   </si>
   <si>
-    <t>§ 275.0-2['(b)(1)']</t>
-  </si>
-  <si>
-    <t>§ 275.0-2['(b)(2)']</t>
-  </si>
-  <si>
     <t>§ 275.0-7['(b)(1)(i)(A)']</t>
   </si>
   <si>
-    <t>documents-2024-12-02-4.json</t>
-  </si>
-  <si>
-    <t>documents-2024-12-02-5.json</t>
-  </si>
-  <si>
-    <t>documents-2024-11-30-1.json</t>
-  </si>
-  <si>
-    <t>documents-2024-11-30-2.json</t>
-  </si>
-  <si>
-    <t>documents-2024-12-01-1.json</t>
-  </si>
-  <si>
-    <t>documents-2024-12-02-1.json</t>
-  </si>
-  <si>
-    <t>documents-2024-12-02-9.json</t>
-  </si>
-  <si>
-    <t>documents-2024-12-02-8.json</t>
-  </si>
-  <si>
-    <t>documents-2024-12-02-6.json</t>
-  </si>
-  <si>
-    <t>documents-2024-11-29-4.json</t>
+    <t>documents-2025-01-11-10.json</t>
+  </si>
+  <si>
+    <t>documents-2025-01-11-9.json</t>
+  </si>
+  <si>
+    <t>documents-2025-01-11-6.json</t>
+  </si>
+  <si>
+    <t>documents-2025-01-11-2.json</t>
+  </si>
+  <si>
+    <t>documents-2025-01-11-1.json</t>
+  </si>
+  <si>
+    <t>documents-2025-01-11-4.json</t>
+  </si>
+  <si>
+    <t>documents-2025-01-11-5.json</t>
+  </si>
+  <si>
+    <t>documents-2025-01-11-7.json</t>
+  </si>
+  <si>
+    <t>documents-2025-01-11-8.json</t>
+  </si>
+  <si>
+    <t>documents-2025-01-11-3.json</t>
   </si>
   <si>
     <t>The Commission will order a hearing on the matter upon its own motion.</t>
   </si>
   <si>
-    <t>Non-resident means an individual who resides in any place not subject to the jurisdiction of the United States.</t>
-  </si>
-  <si>
-    <t>Non-resident means a corporation that is incorporated in or that has its principal office and place of business in any place not subject to the jurisdiction of the United States.</t>
+    <t>The Commission will order a hearing on the matter, upon its own motion.</t>
   </si>
   <si>
     <t>The Commission will order a hearing on the matter upon the request of any interested person.</t>
   </si>
   <si>
+    <t>The Commission will order a hearing on the matter, upon the request of any interested person.</t>
+  </si>
+  <si>
     <t>An investment adviser has assets under management of less than $25 million, or such higher amount as the Commission may by rule deem appropriate under Section 203A(a)(1)(A) of the Act.</t>
   </si>
   <si>
-    <t>Non-resident means a partnership or other unincorporated organization or association that has its principal office and place of business in any place not subject to the jurisdiction of the United States.</t>
-  </si>
-  <si>
     <t>The term small business or small organization for purposes of the Investment Advisers Act of 1940 shall mean an investment adviser that has assets under management of less than $25 million, did not have total assets of $5 million or more on the last day of the most recent fiscal year, and does not control, is not controlled by, and is not under common control with another investment adviser that has assets under management of $25 million or more, or any person that had total assets of $5 million or more on the last day of the most recent fiscal year.</t>
   </si>
   <si>
     <t>An investment adviser does not control, is not controlled by, and is not under common control with another investment adviser that has assets under management of $25 million or more.</t>
   </si>
   <si>
+    <t>A person is presumed to control a corporation if the person directly or indirectly has the right to vote 25 percent or more of a class of the corporation's voting securities, or has the power to sell or direct the sale of 25 percent or more of a class of the corporation's voting securities.</t>
+  </si>
+  <si>
     <t>A person is presumed to control a corporation if the person directly or indirectly has the right to vote 25 percent or more of a class of the corporation's voting securities or has the power to sell or direct the sale of 25 percent or more of a class of the corporation's voting securities.</t>
   </si>
   <si>
-    <t>The Secretary of the Commission will promptly forward a copy to each named party by registered or certified mail at that party's last address filed with the Commission.</t>
-  </si>
-  <si>
     <t>The Secretary of the Commission (Secretary) will promptly forward a copy to each named party by registered or certified mail at that party's last address filed with the Commission.</t>
   </si>
   <si>
@@ -200,12 +182,6 @@
   </si>
   <si>
     <t>The Commission will order a hearing on the matter, if it appears that a hearing is necessary or appropriate in the public interest or for the protection of investors, upon the request of any interested person or upon its own motion.</t>
-  </si>
-  <si>
-    <t>Managing agent means any person, including a trustee, who directs or manages, or who participates in directing or managing, the affairs of any unincorporated organization or association other than a partnership.</t>
-  </si>
-  <si>
-    <t>Non-resident means an individual who resides in any place not subject to the jurisdiction of the United States; a corporation that is incorporated in or that has its principal office and place of business in any place not subject to the jurisdiction of the United States; and a partnership or other unincorporated organization or association that has its principal office and place of business in any place not subject to the jurisdiction of the United States.</t>
   </si>
   <si>
     <t>An investment adviser has assets under management, as defined under Section 203A(a)(3) of the Act and reported on its annual updating amendment to Form ADV, of less than $25 million, or such higher amount as the Commission may by rule deem appropriate.</t>
@@ -584,7 +560,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R33"/>
+  <dimension ref="A1:R35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -666,152 +642,152 @@
         <v>23</v>
       </c>
       <c r="G2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="I2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="J2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="K2">
         <v>0.3017241379310345</v>
       </c>
       <c r="L2" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="M2" t="b">
         <v>1</v>
       </c>
       <c r="N2" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="O2" t="b">
         <v>0</v>
       </c>
       <c r="P2" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="Q2" t="b">
         <v>0</v>
       </c>
       <c r="R2" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:18">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3">
         <v>6</v>
       </c>
       <c r="C3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="H3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="I3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="J3" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="K3">
-        <v>0.3033175355450237</v>
+        <v>0.3017241379310345</v>
       </c>
       <c r="L3" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="M3" t="b">
         <v>1</v>
       </c>
       <c r="N3" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="O3" t="b">
         <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="Q3" t="b">
         <v>0</v>
       </c>
       <c r="R3" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:18">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="H4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="I4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="J4" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="K4">
-        <v>0.3869565217391304</v>
+        <v>0.3017241379310345</v>
       </c>
       <c r="L4" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="M4" t="b">
         <v>1</v>
       </c>
       <c r="N4" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="O4" t="b">
         <v>0</v>
       </c>
       <c r="P4" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="Q4" t="b">
         <v>0</v>
       </c>
       <c r="R4" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:18">
@@ -819,7 +795,7 @@
         <v>18</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -831,272 +807,272 @@
         <v>21</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I5" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="J5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="K5">
-        <v>0.396551724137931</v>
+        <v>0.3060344827586207</v>
       </c>
       <c r="L5" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="M5" t="b">
         <v>1</v>
       </c>
       <c r="N5" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="O5" t="b">
         <v>0</v>
       </c>
       <c r="P5" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="Q5" t="b">
         <v>0</v>
       </c>
       <c r="R5" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:18">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G6" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="H6" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="I6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="J6" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="K6">
-        <v>0.4206349206349206</v>
+        <v>0.396551724137931</v>
       </c>
       <c r="L6" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="M6" t="b">
         <v>1</v>
       </c>
       <c r="N6" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="O6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P6" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="Q6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R6" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:18">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="H7" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="I7" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="J7" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="K7">
-        <v>0.4206349206349206</v>
+        <v>0.396551724137931</v>
       </c>
       <c r="L7" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="M7" t="b">
         <v>1</v>
       </c>
       <c r="N7" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="O7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P7" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="Q7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R7" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:18">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G8" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="H8" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="I8" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="J8" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="K8">
-        <v>0.4206349206349206</v>
+        <v>0.396551724137931</v>
       </c>
       <c r="L8" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="M8" t="b">
         <v>1</v>
       </c>
       <c r="N8" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="O8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P8" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="Q8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R8" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:18">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G9" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="H9" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="I9" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="J9" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="K9">
-        <v>0.4206349206349206</v>
+        <v>0.4008620689655172</v>
       </c>
       <c r="L9" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="M9" t="b">
         <v>1</v>
       </c>
       <c r="N9" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="O9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P9" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="Q9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R9" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:18">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -1111,48 +1087,48 @@
         <v>22</v>
       </c>
       <c r="F10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I10" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="J10" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="K10">
         <v>0.4206349206349206</v>
       </c>
       <c r="L10" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="M10" t="b">
         <v>1</v>
       </c>
       <c r="N10" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="O10" t="b">
         <v>1</v>
       </c>
       <c r="P10" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="Q10" t="b">
         <v>1</v>
       </c>
       <c r="R10" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:18">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -1167,48 +1143,48 @@
         <v>22</v>
       </c>
       <c r="F11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H11" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="I11" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="J11" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="K11">
         <v>0.4206349206349206</v>
       </c>
       <c r="L11" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="M11" t="b">
         <v>1</v>
       </c>
       <c r="N11" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="O11" t="b">
         <v>1</v>
       </c>
       <c r="P11" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="Q11" t="b">
         <v>1</v>
       </c>
       <c r="R11" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:18">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -1223,43 +1199,43 @@
         <v>22</v>
       </c>
       <c r="F12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H12" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="I12" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="J12" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="K12">
         <v>0.4206349206349206</v>
       </c>
       <c r="L12" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="M12" t="b">
         <v>1</v>
       </c>
       <c r="N12" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="O12" t="b">
         <v>1</v>
       </c>
       <c r="P12" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="Q12" t="b">
         <v>1</v>
       </c>
       <c r="R12" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:18">
@@ -1267,10 +1243,10 @@
         <v>19</v>
       </c>
       <c r="B13">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D13" t="s">
         <v>22</v>
@@ -1279,54 +1255,54 @@
         <v>22</v>
       </c>
       <c r="F13" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G13" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="H13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I13" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="J13" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="K13">
-        <v>0.441304347826087</v>
+        <v>0.4206349206349206</v>
       </c>
       <c r="L13" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="M13" t="b">
         <v>1</v>
       </c>
       <c r="N13" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="O13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P13" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="Q13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R13" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:18">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D14" t="s">
         <v>22</v>
@@ -1335,54 +1311,54 @@
         <v>22</v>
       </c>
       <c r="F14" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G14" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="H14" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="I14" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="J14" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="K14">
-        <v>0.4640287769784173</v>
+        <v>0.4206349206349206</v>
       </c>
       <c r="L14" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="M14" t="b">
         <v>1</v>
       </c>
       <c r="N14" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="O14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P14" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="Q14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R14" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:18">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C15">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D15" t="s">
         <v>22</v>
@@ -1391,54 +1367,54 @@
         <v>22</v>
       </c>
       <c r="F15" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G15" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="H15" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="I15" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="J15" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="K15">
-        <v>0.5723270440251572</v>
+        <v>0.4206349206349206</v>
       </c>
       <c r="L15" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="M15" t="b">
         <v>1</v>
       </c>
       <c r="N15" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="O15" t="b">
         <v>1</v>
       </c>
       <c r="P15" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="Q15" t="b">
         <v>1</v>
       </c>
       <c r="R15" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:18">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C16">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D16" t="s">
         <v>22</v>
@@ -1447,51 +1423,51 @@
         <v>22</v>
       </c>
       <c r="F16" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G16" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="H16" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="I16" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="J16" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="K16">
-        <v>0.5723270440251572</v>
+        <v>0.4206349206349206</v>
       </c>
       <c r="L16" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="M16" t="b">
         <v>1</v>
       </c>
       <c r="N16" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="O16" t="b">
         <v>1</v>
       </c>
       <c r="P16" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="Q16" t="b">
         <v>1</v>
       </c>
       <c r="R16" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:18">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C17">
         <v>4</v>
@@ -1503,51 +1479,51 @@
         <v>22</v>
       </c>
       <c r="F17" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G17" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I17" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="J17" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="K17">
-        <v>0.5723270440251572</v>
+        <v>0.4640287769784173</v>
       </c>
       <c r="L17" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="M17" t="b">
         <v>1</v>
       </c>
       <c r="N17" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="O17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P17" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="Q17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R17" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:18">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C18">
         <v>4</v>
@@ -1559,51 +1535,51 @@
         <v>22</v>
       </c>
       <c r="F18" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G18" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H18" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="I18" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="J18" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="K18">
-        <v>0.5723270440251572</v>
+        <v>0.4640287769784173</v>
       </c>
       <c r="L18" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="M18" t="b">
         <v>1</v>
       </c>
       <c r="N18" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="O18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P18" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="Q18" t="b">
         <v>0</v>
       </c>
       <c r="R18" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:18">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C19">
         <v>4</v>
@@ -1615,51 +1591,51 @@
         <v>22</v>
       </c>
       <c r="F19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G19" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H19" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I19" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="J19" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="K19">
-        <v>0.5723270440251572</v>
+        <v>0.4640287769784173</v>
       </c>
       <c r="L19" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="M19" t="b">
         <v>1</v>
       </c>
       <c r="N19" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="O19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P19" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="Q19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R19" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:18">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C20">
         <v>4</v>
@@ -1671,48 +1647,48 @@
         <v>22</v>
       </c>
       <c r="F20" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G20" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H20" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="I20" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="J20" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="K20">
-        <v>0.5723270440251572</v>
+        <v>0.4640287769784173</v>
       </c>
       <c r="L20" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="M20" t="b">
         <v>1</v>
       </c>
       <c r="N20" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="O20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P20" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="Q20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R20" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:18">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>4</v>
@@ -1727,99 +1703,99 @@
         <v>22</v>
       </c>
       <c r="F21" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G21" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H21" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I21" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="J21" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="K21">
         <v>0.5723270440251572</v>
       </c>
       <c r="L21" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="M21" t="b">
         <v>1</v>
       </c>
       <c r="N21" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="O21" t="b">
         <v>1</v>
       </c>
       <c r="P21" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="Q21" t="b">
         <v>1</v>
       </c>
       <c r="R21" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:18">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C22">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E22" t="s">
         <v>22</v>
       </c>
       <c r="F22" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G22" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="H22" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="I22" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="J22" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="K22">
-        <v>0.6</v>
+        <v>0.5723270440251572</v>
       </c>
       <c r="L22" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="M22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N22" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="O22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P22" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="Q22" t="b">
         <v>0</v>
       </c>
       <c r="R22" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:18">
@@ -1827,55 +1803,55 @@
         <v>19</v>
       </c>
       <c r="B23">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C23">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E23" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F23" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="G23" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="H23" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I23" t="s">
+        <v>49</v>
+      </c>
+      <c r="J23" t="s">
         <v>57</v>
       </c>
-      <c r="J23" t="s">
-        <v>67</v>
-      </c>
       <c r="K23">
-        <v>0.6007194244604317</v>
+        <v>0.5723270440251572</v>
       </c>
       <c r="L23" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="M23" t="b">
         <v>1</v>
       </c>
       <c r="N23" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="O23" t="b">
         <v>1</v>
       </c>
       <c r="P23" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="Q23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R23" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:18">
@@ -1883,55 +1859,55 @@
         <v>19</v>
       </c>
       <c r="B24">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C24">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E24" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F24" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="G24" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="H24" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I24" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="J24" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="K24">
-        <v>0.6438848920863309</v>
+        <v>0.5723270440251572</v>
       </c>
       <c r="L24" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="M24" t="b">
         <v>1</v>
       </c>
       <c r="N24" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="O24" t="b">
         <v>1</v>
       </c>
       <c r="P24" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="Q24" t="b">
         <v>1</v>
       </c>
       <c r="R24" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:18">
@@ -1939,55 +1915,55 @@
         <v>19</v>
       </c>
       <c r="B25">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C25">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D25" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E25" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F25" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G25" t="s">
         <v>32</v>
       </c>
       <c r="H25" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="I25" t="s">
+        <v>50</v>
+      </c>
+      <c r="J25" t="s">
         <v>58</v>
       </c>
-      <c r="J25" t="s">
-        <v>67</v>
-      </c>
       <c r="K25">
-        <v>0.6438848920863309</v>
+        <v>0.5979381443298969</v>
       </c>
       <c r="L25" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="M25" t="b">
         <v>1</v>
       </c>
       <c r="N25" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="O25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P25" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="Q25" t="b">
         <v>1</v>
       </c>
       <c r="R25" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:18">
@@ -1995,55 +1971,55 @@
         <v>19</v>
       </c>
       <c r="B26">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C26">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D26" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E26" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F26" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G26" t="s">
         <v>32</v>
       </c>
       <c r="H26" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="I26" t="s">
+        <v>50</v>
+      </c>
+      <c r="J26" t="s">
         <v>58</v>
       </c>
-      <c r="J26" t="s">
-        <v>67</v>
-      </c>
       <c r="K26">
-        <v>0.6438848920863309</v>
+        <v>0.5979381443298969</v>
       </c>
       <c r="L26" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="M26" t="b">
         <v>1</v>
       </c>
       <c r="N26" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="O26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P26" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="Q26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R26" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:18">
@@ -2051,63 +2027,63 @@
         <v>19</v>
       </c>
       <c r="B27">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C27">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D27" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E27" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F27" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G27" t="s">
         <v>32</v>
       </c>
       <c r="H27" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="I27" t="s">
+        <v>51</v>
+      </c>
+      <c r="J27" t="s">
         <v>58</v>
       </c>
-      <c r="J27" t="s">
-        <v>67</v>
-      </c>
       <c r="K27">
-        <v>0.6438848920863309</v>
+        <v>0.6</v>
       </c>
       <c r="L27" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="M27" t="b">
         <v>1</v>
       </c>
       <c r="N27" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="O27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P27" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="Q27" t="b">
         <v>0</v>
       </c>
       <c r="R27" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:18">
       <c r="A28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B28">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C28">
         <v>6</v>
@@ -2119,43 +2095,43 @@
         <v>22</v>
       </c>
       <c r="F28" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G28" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="H28" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I28" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="J28" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="K28">
-        <v>0.7103825136612022</v>
+        <v>0.6</v>
       </c>
       <c r="L28" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="M28" t="b">
         <v>1</v>
       </c>
       <c r="N28" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="O28" t="b">
         <v>0</v>
       </c>
       <c r="P28" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="Q28" t="b">
         <v>0</v>
       </c>
       <c r="R28" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:18">
@@ -2163,66 +2139,66 @@
         <v>20</v>
       </c>
       <c r="B29">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C29">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D29" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E29" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F29" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G29" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="H29" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="I29" t="s">
+        <v>52</v>
+      </c>
+      <c r="J29" t="s">
         <v>59</v>
       </c>
-      <c r="J29" t="s">
-        <v>66</v>
-      </c>
       <c r="K29">
-        <v>0.7103825136612022</v>
+        <v>0.6438848920863309</v>
       </c>
       <c r="L29" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="M29" t="b">
         <v>1</v>
       </c>
       <c r="N29" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="O29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P29" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="Q29" t="b">
         <v>0</v>
       </c>
       <c r="R29" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:18">
       <c r="A30" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B30">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C30">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D30" t="s">
         <v>21</v>
@@ -2231,99 +2207,99 @@
         <v>21</v>
       </c>
       <c r="F30" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G30" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I30" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="J30" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K30">
-        <v>0.7155172413793103</v>
+        <v>0.6438848920863309</v>
       </c>
       <c r="L30" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="M30" t="b">
         <v>1</v>
       </c>
       <c r="N30" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="O30" t="b">
         <v>1</v>
       </c>
       <c r="P30" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="Q30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R30" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:18">
       <c r="A31" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B31">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C31">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D31" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E31" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F31" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G31" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H31" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="I31" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="J31" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="K31">
-        <v>0.7155172413793103</v>
+        <v>0.7103825136612022</v>
       </c>
       <c r="L31" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="M31" t="b">
         <v>1</v>
       </c>
       <c r="N31" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="O31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P31" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="Q31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R31" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:18">
@@ -2343,43 +2319,43 @@
         <v>21</v>
       </c>
       <c r="F32" t="s">
+        <v>31</v>
+      </c>
+      <c r="G32" t="s">
+        <v>31</v>
+      </c>
+      <c r="H32" t="s">
         <v>34</v>
       </c>
-      <c r="G32" t="s">
-        <v>34</v>
-      </c>
-      <c r="H32" t="s">
-        <v>38</v>
-      </c>
       <c r="I32" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="J32" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="K32">
         <v>0.7155172413793103</v>
       </c>
       <c r="L32" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="M32" t="b">
         <v>1</v>
       </c>
       <c r="N32" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="O32" t="b">
         <v>1</v>
       </c>
       <c r="P32" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="Q32" t="b">
         <v>1</v>
       </c>
       <c r="R32" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:18">
@@ -2399,43 +2375,155 @@
         <v>21</v>
       </c>
       <c r="F33" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G33" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H33" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="I33" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="J33" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="K33">
         <v>0.7155172413793103</v>
       </c>
       <c r="L33" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="M33" t="b">
         <v>1</v>
       </c>
       <c r="N33" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="O33" t="b">
         <v>1</v>
       </c>
       <c r="P33" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="Q33" t="b">
         <v>1</v>
       </c>
       <c r="R33" t="s">
-        <v>69</v>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18">
+      <c r="A34" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34">
+        <v>4</v>
+      </c>
+      <c r="C34">
+        <v>4</v>
+      </c>
+      <c r="D34" t="s">
+        <v>21</v>
+      </c>
+      <c r="E34" t="s">
+        <v>21</v>
+      </c>
+      <c r="F34" t="s">
+        <v>31</v>
+      </c>
+      <c r="G34" t="s">
+        <v>31</v>
+      </c>
+      <c r="H34" t="s">
+        <v>36</v>
+      </c>
+      <c r="I34" t="s">
+        <v>54</v>
+      </c>
+      <c r="J34" t="s">
+        <v>55</v>
+      </c>
+      <c r="K34">
+        <v>0.7155172413793103</v>
+      </c>
+      <c r="L34" t="s">
+        <v>60</v>
+      </c>
+      <c r="M34" t="b">
+        <v>1</v>
+      </c>
+      <c r="N34" t="s">
+        <v>61</v>
+      </c>
+      <c r="O34" t="b">
+        <v>1</v>
+      </c>
+      <c r="P34" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q34" t="b">
+        <v>1</v>
+      </c>
+      <c r="R34" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18">
+      <c r="A35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35">
+        <v>4</v>
+      </c>
+      <c r="C35">
+        <v>4</v>
+      </c>
+      <c r="D35" t="s">
+        <v>21</v>
+      </c>
+      <c r="E35" t="s">
+        <v>21</v>
+      </c>
+      <c r="F35" t="s">
+        <v>31</v>
+      </c>
+      <c r="G35" t="s">
+        <v>31</v>
+      </c>
+      <c r="H35" t="s">
+        <v>33</v>
+      </c>
+      <c r="I35" t="s">
+        <v>54</v>
+      </c>
+      <c r="J35" t="s">
+        <v>55</v>
+      </c>
+      <c r="K35">
+        <v>0.7155172413793103</v>
+      </c>
+      <c r="L35" t="s">
+        <v>60</v>
+      </c>
+      <c r="M35" t="b">
+        <v>1</v>
+      </c>
+      <c r="N35" t="s">
+        <v>61</v>
+      </c>
+      <c r="O35" t="b">
+        <v>1</v>
+      </c>
+      <c r="P35" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q35" t="b">
+        <v>1</v>
+      </c>
+      <c r="R35" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>